<commit_message>
UPDATE: jsons & xlsx
</commit_message>
<xml_diff>
--- a/data/common/excel/PUBLIC_CATEGORY_SKU.xlsx
+++ b/data/common/excel/PUBLIC_CATEGORY_SKU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OPT Design\PycharmProjects\optima-scrapper\data\common\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9439CD97-512C-4115-9F57-B5F28A4FE79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449FB151-AD86-4985-AC47-849346F645B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98414BF8-B91D-4538-8B60-2AD3F6A6ADCC}"/>
   </bookViews>
@@ -498,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="51">
+  <fills count="52">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -799,6 +799,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -827,7 +833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -893,7 +899,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="51" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1226,20 +1235,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF40A98-2910-49B0-BB76-BAF76F0B7575}">
   <dimension ref="A1:C4836"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4799" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4746" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="56"/>
+    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="56" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="58" t="s">
         <v>143</v>
       </c>
       <c r="C1" s="57" t="s">
@@ -54441,7 +54452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB99A47F-7B2A-40D1-9D34-AD0055C02F9B}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView zoomScale="226" zoomScaleNormal="226" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="226" zoomScaleNormal="226" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
UPDATE: corrected excel column naming
</commit_message>
<xml_diff>
--- a/data/common/excel/PUBLIC_CATEGORY_SKU.xlsx
+++ b/data/common/excel/PUBLIC_CATEGORY_SKU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OPT Design\PycharmProjects\optima-scrapper\data\common\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449FB151-AD86-4985-AC47-849346F645B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F788AF9B-15FD-439F-8F79-FA187F8335C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98414BF8-B91D-4538-8B60-2AD3F6A6ADCC}"/>
   </bookViews>
@@ -457,10 +457,10 @@
     <t>SOLAR ENERGY</t>
   </si>
   <si>
-    <t>CATEGORIAS INGLES</t>
+    <t>CATEGORY ES</t>
   </si>
   <si>
-    <t>CATEGORIAS ESPAÑOL</t>
+    <t>CATEGORY EN</t>
   </si>
 </sst>
 </file>
@@ -896,7 +896,7 @@
     <xf numFmtId="0" fontId="1" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="51" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF40A98-2910-49B0-BB76-BAF76F0B7575}">
   <dimension ref="A1:C4836"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4799" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4746" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,10 +1248,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="58" t="s">
         <v>144</v>
-      </c>
-      <c r="B1" s="58" t="s">
-        <v>143</v>
       </c>
       <c r="C1" s="57" t="s">
         <v>2</v>

</xml_diff>